<commit_message>
final project 3 work
</commit_message>
<xml_diff>
--- a/Project3/vectorData.xlsx
+++ b/Project3/vectorData.xlsx
@@ -359,7 +359,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>0.52758702082347575</v>
+        <v>0.52758702082347608</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -369,42 +369,42 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1.2439188373410124</v>
+        <v>1.2439188373410155</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>0.5473136227606118</v>
+        <v>0.54731362276061346</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>0.99254849028778525</v>
+        <v>0.99254849028778724</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1.3879273326255566</v>
+        <v>1.3879273326255563</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>0.5473136227606118</v>
+        <v>0.54731362276061346</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>0.91694280083408641</v>
+        <v>0.91694280083408841</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1.0110079158022276</v>
+        <v>1.0110079158022289</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>0.44327178513447185</v>
+        <v>0.44327178513447063</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
@@ -414,67 +414,67 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>0.53174346445651099</v>
+        <v>0.53174346445651</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>0.58251725542081256</v>
+        <v>0.58251725542081312</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>0.42833465256266456</v>
+        <v>0.42833465256266601</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>0.42085701220488714</v>
+        <v>0.42085701220488492</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>0.41361798387089793</v>
+        <v>0.41361798387089649</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>0.54817658381784262</v>
+        <v>0.54817658381784051</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>0.40504274014404601</v>
+        <v>0.40504274014404518</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>0.39996409433708568</v>
+        <v>0.39996409433708469</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>0.13667023651898472</v>
+        <v>0.13667023651898422</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>0.22897071122088192</v>
+        <v>0.22897071122088142</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>0.23870416478277792</v>
+        <v>0.23870416478277678</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>0.10509262880868073</v>
+        <v>0.10509262880868125</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>0.10695987792107606</v>
+        <v>0.10695987792107532</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
@@ -484,42 +484,42 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>0.46186184904713395</v>
+        <v>0.46186184904713229</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>0.13667023651898472</v>
+        <v>0.13667023651898422</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>0.41758010486210334</v>
+        <v>0.41758010486210134</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>3.5327416120882027E-2</v>
+        <v>3.5327416120881985E-2</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>0.60566661926853527</v>
+        <v>0.60566661926853627</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>2.0551178900621494</v>
+        <v>2.0551178900621458</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>0.53122030610965643</v>
+        <v>0.53122030610965598</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>0.54628238816215235</v>
+        <v>0.54628238816215369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>